<commit_message>
Uppercase and escape char test added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilirahmeti/Documents/test/Airspace/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilirahmeti/Documents/test/github_projects/Airspace/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E515CAEB-4041-3645-921B-A3AC0312C455}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895070FB-FDAD-764F-BAE7-133A235B50BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{F9A2BB30-64F1-A044-A18E-D98963208A7D}"/>
+    <workbookView xWindow="4280" yWindow="3560" windowWidth="28040" windowHeight="17440" xr2:uid="{F9A2BB30-64F1-A044-A18E-D98963208A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
   <si>
     <t>JohnDoe@</t>
   </si>
@@ -232,11 +232,6 @@
     <t>or true--</t>
   </si>
   <si>
-    <t xml:space="preserve"> or true--
-' or true--
-) or true--</t>
-  </si>
-  <si>
     <t>' or 'x'='x</t>
   </si>
   <si>
@@ -253,6 +248,84 @@
   </si>
   <si>
     <t>)) or ((x"))=(("x</t>
+  </si>
+  <si>
+    <t>' or true--</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> or true--</t>
+  </si>
+  <si>
+    <t>) or true--</t>
+  </si>
+  <si>
+    <t>escaped Character username</t>
+  </si>
+  <si>
+    <t>escaped Character password</t>
+  </si>
+  <si>
+    <t>o&amp;apos;neil</t>
+  </si>
+  <si>
+    <t>o&amp;amp;neil</t>
+  </si>
+  <si>
+    <t>o&amp;lt;neil</t>
+  </si>
+  <si>
+    <t>o&amp;gt;neil</t>
+  </si>
+  <si>
+    <t>o&amp;quot;neil</t>
+  </si>
+  <si>
+    <t>Uppercase username</t>
+  </si>
+  <si>
+    <t>Uppercase password</t>
+  </si>
+  <si>
+    <t>TOMSMITH</t>
+  </si>
+  <si>
+    <t>SuperSecretPassword!</t>
+  </si>
+  <si>
+    <t>SUPERSECRETPASSWORD!</t>
+  </si>
+  <si>
+    <t>tomsmith</t>
+  </si>
+  <si>
+    <t>TomSMITH</t>
+  </si>
+  <si>
+    <t>Tomsmith</t>
+  </si>
+  <si>
+    <t>TOMsmith</t>
+  </si>
+  <si>
+    <t>TomSmith</t>
+  </si>
+  <si>
+    <t>supersecretpassword!</t>
+  </si>
+  <si>
+    <t>SUPERsecretpassword!</t>
+  </si>
+  <si>
+    <t>SUPERSECRETpassword!</t>
+  </si>
+  <si>
+    <t>tom smith</t>
+  </si>
+  <si>
+    <t>superSECRETpassword!</t>
+  </si>
+  <si>
+    <t>super SecretPassword!</t>
   </si>
 </sst>
 </file>
@@ -622,15 +695,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C8CB4C-1B7B-7F44-A2A4-ACDED5B9735B}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -643,8 +724,20 @@
       <c r="D1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,8 +750,20 @@
       <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -671,8 +776,20 @@
       <c r="D3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -685,8 +802,20 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -699,8 +828,20 @@
       <c r="D5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -713,8 +854,20 @@
       <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -727,8 +880,14 @@
       <c r="D7" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -741,8 +900,14 @@
       <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -755,8 +920,14 @@
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -769,8 +940,14 @@
       <c r="D10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -783,8 +960,14 @@
       <c r="D11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -797,8 +980,14 @@
       <c r="D12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -811,8 +1000,14 @@
       <c r="D13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -825,8 +1020,14 @@
       <c r="D14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -840,7 +1041,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -974,10 +1175,10 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1100,12 +1301,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1118,42 +1319,58 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C40" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>